<commit_message>
Modified The Main For paper Generation
</commit_message>
<xml_diff>
--- a/Q#.xlsx
+++ b/Q#.xlsx
@@ -590,6 +590,11 @@
           <t>BATCH</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="12.8" customHeight="1" s="8">
       <c r="A7" s="12" t="inlineStr">
@@ -597,10 +602,18 @@
           <t>COURSE</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Mathematics</t>
+        </is>
+      </c>
       <c r="F7" s="12" t="inlineStr">
         <is>
           <t>MAX MARKS</t>
         </is>
+      </c>
+      <c r="G7" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="8" ht="12.8" customHeight="1" s="8">
@@ -609,6 +622,11 @@
           <t>COURSE CODE</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>201</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="12.8" customHeight="1" s="8">
       <c r="A9" s="12" t="inlineStr">
@@ -616,6 +634,11 @@
           <t xml:space="preserve">DATE AND TIME: </t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>12/12/2023</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="12.8" customHeight="1" s="8">
       <c r="A11" s="12" t="inlineStr">
@@ -661,7 +684,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>What is Probability ?</t>
+          <t>Define Probability ?</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -678,7 +701,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>What Is head Probability in tossing a coin ?</t>
+          <t>A coin is tossed twice find the probability of getting alteast head ?</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">

</xml_diff>